<commit_message>
Bioc style check fixes v2
</commit_message>
<xml_diff>
--- a/inst/extdata/ega_full_template_v2.xlsx
+++ b/inst/extdata/ega_full_template_v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/igor/_DBM/projects/rega_package/Rega/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A53F86FE-6E9D-0E4F-8CFE-6098AF679042}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15B1F8B5-A830-6544-81AC-73266CF6DD1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="11" xr2:uid="{C6701382-EF30-1B43-A607-1356FE361260}"/>
+    <workbookView xWindow="51200" yWindow="9920" windowWidth="30240" windowHeight="18880" activeTab="4" xr2:uid="{C6701382-EF30-1B43-A607-1356FE361260}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="7" r:id="rId1"/>
@@ -3763,7 +3763,7 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -5474,8 +5474,8 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Updated xlsx template, set new parser defaults
</commit_message>
<xml_diff>
--- a/inst/extdata/ega_full_template_v2.xlsx
+++ b/inst/extdata/ega_full_template_v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/igor/_DBM/projects/rega_package/Rega/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15B1F8B5-A830-6544-81AC-73266CF6DD1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A18B514A-C117-5540-9888-E783F5F5DA7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="9920" windowWidth="30240" windowHeight="18880" activeTab="4" xr2:uid="{C6701382-EF30-1B43-A607-1356FE361260}"/>
+    <workbookView xWindow="51200" yWindow="9920" windowWidth="30240" windowHeight="18880" xr2:uid="{C6701382-EF30-1B43-A607-1356FE361260}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="7" r:id="rId1"/>
@@ -669,7 +669,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="469">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="453">
   <si>
     <t>Description</t>
   </si>
@@ -1917,9 +1917,6 @@
   </si>
   <si>
     <t>Here you describe your dataset(s).</t>
-  </si>
-  <si>
-    <t>Dataset description is expected to be a 3-4 sentences definition of the dataset content, including sample number and details, file type, and technology/experimentation used.</t>
   </si>
   <si>
     <t>Additional Instructions</t>
@@ -2205,57 +2202,6 @@
     </r>
   </si>
   <si>
-    <t>Experiment2</t>
-  </si>
-  <si>
-    <t>Dataset2</t>
-  </si>
-  <si>
-    <t>Dataset3</t>
-  </si>
-  <si>
-    <t>Sample2</t>
-  </si>
-  <si>
-    <t>Sample3</t>
-  </si>
-  <si>
-    <t>Sample4</t>
-  </si>
-  <si>
-    <t>Sample5</t>
-  </si>
-  <si>
-    <t>Sample6</t>
-  </si>
-  <si>
-    <t>Sample7</t>
-  </si>
-  <si>
-    <t>Sample8</t>
-  </si>
-  <si>
-    <t>Sample9</t>
-  </si>
-  <si>
-    <t>Sample10</t>
-  </si>
-  <si>
-    <t>Analysis2</t>
-  </si>
-  <si>
-    <t>Run2</t>
-  </si>
-  <si>
-    <t>Run3</t>
-  </si>
-  <si>
-    <t>Run4</t>
-  </si>
-  <si>
-    <t>Run5</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">For </t>
     </r>
@@ -2328,6 +2274,12 @@
   </si>
   <si>
     <t>* Access Type</t>
+  </si>
+  <si>
+    <t>Dataset description is expected to be a 3-4 sentences (at least 50 characters), definition of the dataset content, including sample number and details, file type, and technology/experimentation used.</t>
+  </si>
+  <si>
+    <t>Files cannot be reused among the different Runs. Each file can only be associated to one Run.</t>
   </si>
 </sst>
 </file>
@@ -2721,13 +2673,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>76</xdr:row>
+      <xdr:row>77</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>83</xdr:row>
+      <xdr:row>84</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3107,10 +3059,10 @@
   <sheetPr>
     <tabColor theme="0"/>
   </sheetPr>
-  <dimension ref="A1:D75"/>
+  <dimension ref="A1:D76"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3129,27 +3081,27 @@
     <row r="2" spans="1:2" ht="18" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="39" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="B4" s="5" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="B5" s="5" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="B7" s="5" t="s">
-        <v>463</v>
+        <v>445</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="18" x14ac:dyDescent="0.2"/>
@@ -3168,44 +3120,44 @@
     </row>
     <row r="18" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="B18" s="5" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="B19" s="5" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="B20" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="18" x14ac:dyDescent="0.2"/>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="39" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="39"/>
       <c r="B23" s="5" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="B24" s="5" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="B25" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="B26" s="5" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="18" x14ac:dyDescent="0.2"/>
@@ -3216,7 +3168,7 @@
     </row>
     <row r="29" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="B29" s="5" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="18" x14ac:dyDescent="0.2"/>
@@ -3248,12 +3200,12 @@
     </row>
     <row r="37" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="B37" s="5" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="B38" s="5" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="18" x14ac:dyDescent="0.2"/>
@@ -3264,7 +3216,7 @@
     </row>
     <row r="41" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="B41" s="9" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="18" x14ac:dyDescent="0.2">
@@ -3317,126 +3269,131 @@
     </row>
     <row r="49" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="B49" s="5" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="B50" s="40"/>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" s="39" t="s">
+      <c r="B50" s="5" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="B51" s="40"/>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" s="39" t="s">
         <v>383</v>
       </c>
-      <c r="B51" s="40"/>
-    </row>
-    <row r="52" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="B52" s="5" t="s">
-        <v>428</v>
-      </c>
+      <c r="B52" s="40"/>
     </row>
     <row r="53" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="B53" s="5" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="B54" s="5" t="s">
-        <v>467</v>
+        <v>428</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="B55" s="5" t="s">
-        <v>465</v>
+        <v>449</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="B56" s="5" t="s">
-        <v>464</v>
+        <v>447</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="B57" s="5" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" ht="18" x14ac:dyDescent="0.2"/>
-    <row r="59" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="39" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="B58" s="5" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="18" x14ac:dyDescent="0.2"/>
+    <row r="60" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="39" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="B60" s="9" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="B61" s="9" t="s">
-        <v>438</v>
+        <v>415</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="B62" s="9" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" ht="18" x14ac:dyDescent="0.2"/>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A64" s="39" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="B65" s="5" t="s">
-        <v>436</v>
+        <v>437</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="B63" s="9" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="18" x14ac:dyDescent="0.2"/>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" s="39" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="B66" s="5" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" ht="18" x14ac:dyDescent="0.2"/>
-    <row r="68" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="39" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="B69" s="5" t="s">
-        <v>430</v>
+        <v>435</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="B67" s="5" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="18" x14ac:dyDescent="0.2"/>
+    <row r="69" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="39" t="s">
+        <v>416</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="B70" s="5" t="s">
-        <v>462</v>
+        <v>429</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="B71" s="5" t="s">
-        <v>418</v>
+        <v>444</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="B72" s="5" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="B73" s="5" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A74" s="42"/>
+      <c r="B74" s="42" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A73" s="42"/>
-      <c r="B73" s="42" t="s">
+    <row r="75" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A75" s="43"/>
+      <c r="B75" s="43" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="B76" s="5" t="s">
         <v>420</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A74" s="43"/>
-      <c r="B74" s="43" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="B75" s="5" t="s">
-        <v>421</v>
       </c>
     </row>
   </sheetData>
@@ -3778,7 +3735,7 @@
         <v>175</v>
       </c>
       <c r="B1" s="32" t="s">
-        <v>468</v>
+        <v>450</v>
       </c>
       <c r="C1" s="32" t="s">
         <v>174</v>
@@ -5087,10 +5044,10 @@
   <sheetPr>
     <tabColor rgb="FF603E24"/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5139,75 +5096,6 @@
       </c>
       <c r="F2" s="2" t="s">
         <v>384</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="2" t="s">
-        <v>445</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>446</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>448</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C4" s="2" t="s">
-        <v>447</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>449</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D5" s="2" t="s">
-        <v>450</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D6" s="2" t="s">
-        <v>451</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D7" s="2" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D8" s="2" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D9" s="2" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D10" s="2" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D11" s="2" t="s">
-        <v>456</v>
       </c>
     </row>
   </sheetData>
@@ -5474,7 +5362,7 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>

</xml_diff>